<commit_message>
Correct call from page Préfecture
</commit_message>
<xml_diff>
--- a/runtime/apps/delphes/delphes.xlsx
+++ b/runtime/apps/delphes/delphes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\runtime\apps\delphes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6E22C7-D566-418F-9669-DCC25987BE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6005BC64-7D16-40EC-80CD-BEFC71EC1E28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="973" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="973" firstSheet="4" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -1043,7 +1043,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1064,6 +1064,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1097,7 +1103,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1145,6 +1151,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1447,7 +1457,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:C6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1842,7 +1852,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1931,7 +1941,7 @@
       <c r="E4" s="14" t="s">
         <v>257</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="23" t="s">
         <v>272</v>
       </c>
     </row>
@@ -1966,7 +1976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
@@ -2067,7 +2077,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
@@ -2157,7 +2167,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2458,7 +2468,7 @@
       <c r="D19" s="7" t="s">
         <v>303</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="24" t="s">
         <v>304</v>
       </c>
     </row>
@@ -2475,7 +2485,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2524,7 +2534,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2619,7 +2629,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="O33" sqref="O33"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2683,7 +2693,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2756,7 +2766,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3394,7 +3404,7 @@
   <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Change delphes.xlsx to not send email from Scaleway
</commit_message>
<xml_diff>
--- a/runtime/apps/delphes/delphes.xlsx
+++ b/runtime/apps/delphes/delphes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10824"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\athena\github\trusted-service\runtime\apps\delphes\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime/apps/delphes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5793269-EE19-4E6D-AE73-2801FB792B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EA5BFEA-909D-664F-9FD2-82B211D3D3E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="973" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="760" windowWidth="34680" windowHeight="15720" tabRatio="973" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -1148,9 +1148,9 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Satisfaisant" xfId="1" builtinId="26"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1437,7 +1437,7 @@
       <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1451,32 +1451,32 @@
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="60" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="49.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="40.5703125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="49.7109375" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="2" max="2" width="40.5" style="1" customWidth="1"/>
+    <col min="3" max="3" width="49.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="40.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="49.6640625" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
@@ -1493,7 +1493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>43</v>
       </c>
@@ -1510,7 +1510,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>44</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>217</v>
       </c>
@@ -1544,7 +1544,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>45</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
         <v>46</v>
       </c>
@@ -1578,7 +1578,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>223</v>
       </c>
@@ -1595,7 +1595,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>216</v>
       </c>
@@ -1612,7 +1612,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>214</v>
       </c>
@@ -1629,7 +1629,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>215</v>
       </c>
@@ -1646,7 +1646,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
         <v>218</v>
       </c>
@@ -1663,7 +1663,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
         <v>225</v>
       </c>
@@ -1680,7 +1680,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>222</v>
       </c>
@@ -1697,7 +1697,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
         <v>226</v>
       </c>
@@ -1714,7 +1714,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
         <v>227</v>
       </c>
@@ -1731,7 +1731,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
         <v>224</v>
       </c>
@@ -1748,7 +1748,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
         <v>221</v>
       </c>
@@ -1765,7 +1765,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
         <v>234</v>
       </c>
@@ -1782,7 +1782,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
         <v>219</v>
       </c>
@@ -1799,7 +1799,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
         <v>220</v>
       </c>
@@ -1832,7 +1832,7 @@
       <selection activeCell="V30" sqref="V30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1846,17 +1846,17 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="41.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.5703125" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="41.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -1876,7 +1876,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>267</v>
       </c>
@@ -1896,7 +1896,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>269</v>
       </c>
@@ -1916,7 +1916,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>270</v>
       </c>
@@ -1957,7 +1957,7 @@
       <selection activeCell="X25" sqref="X25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1967,18 +1967,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="24.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1989,7 +1989,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>93</v>
       </c>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>94</v>
       </c>
@@ -2007,7 +2007,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>92</v>
       </c>
@@ -2016,7 +2016,7 @@
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>86</v>
       </c>
@@ -2025,7 +2025,7 @@
       </c>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>87</v>
       </c>
@@ -2034,7 +2034,7 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>90</v>
       </c>
@@ -2043,12 +2043,12 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>189</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>188</v>
@@ -2072,15 +2072,15 @@
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.7109375" customWidth="1"/>
+    <col min="1" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="101" customWidth="1"/>
-    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="4" max="4" width="21.6640625" customWidth="1"/>
     <col min="5" max="5" width="101" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>3</v>
       </c>
@@ -2097,7 +2097,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>103</v>
       </c>
@@ -2114,7 +2114,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>104</v>
       </c>
@@ -2147,7 +2147,7 @@
       <selection activeCell="W28" sqref="W28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2161,20 +2161,20 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -2191,7 +2191,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
         <v>124</v>
       </c>
@@ -2208,7 +2208,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
         <v>125</v>
       </c>
@@ -2225,7 +2225,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
         <v>126</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>127</v>
       </c>
@@ -2259,7 +2259,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>278</v>
       </c>
@@ -2276,7 +2276,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
         <v>276</v>
       </c>
@@ -2293,7 +2293,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
         <v>279</v>
       </c>
@@ -2310,7 +2310,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
         <v>238</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
         <v>240</v>
       </c>
@@ -2344,7 +2344,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>242</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>284</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
         <v>285</v>
       </c>
@@ -2395,7 +2395,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>286</v>
       </c>
@@ -2412,7 +2412,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>292</v>
       </c>
@@ -2429,7 +2429,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>293</v>
       </c>
@@ -2446,7 +2446,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>294</v>
       </c>
@@ -2463,7 +2463,7 @@
         <v>299</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H31" s="20"/>
     </row>
   </sheetData>
@@ -2479,14 +2479,14 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="100.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="101.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="100.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="101.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2497,7 +2497,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>259</v>
       </c>
@@ -2506,7 +2506,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>300</v>
       </c>
@@ -2524,18 +2524,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549C78AA-1218-455B-9887-3E0A5E59C6C7}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.42578125" customWidth="1"/>
-    <col min="2" max="2" width="210.7109375" customWidth="1"/>
-    <col min="3" max="3" width="129.85546875" customWidth="1"/>
+    <col min="1" max="1" width="35.5" customWidth="1"/>
+    <col min="2" max="2" width="210.6640625" customWidth="1"/>
+    <col min="3" max="3" width="129.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>99</v>
       </c>
@@ -2555,7 +2555,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>186</v>
       </c>
@@ -2564,7 +2564,7 @@
       </c>
       <c r="C3" s="5"/>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>187</v>
       </c>
@@ -2573,7 +2573,7 @@
       </c>
       <c r="C4" s="5"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>184</v>
       </c>
@@ -2582,7 +2582,7 @@
       </c>
       <c r="C5" s="5"/>
     </row>
-    <row r="6" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>185</v>
       </c>
@@ -2591,7 +2591,7 @@
       </c>
       <c r="C6" s="5"/>
     </row>
-    <row r="7" spans="1:3" ht="225" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>257</v>
       </c>
@@ -2600,7 +2600,7 @@
       </c>
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="1:3" ht="240" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>258</v>
       </c>
@@ -2623,14 +2623,14 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="38.28515625" customWidth="1"/>
-    <col min="2" max="2" width="29.28515625" customWidth="1"/>
+    <col min="1" max="1" width="38.33203125" customWidth="1"/>
+    <col min="2" max="2" width="29.33203125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>191</v>
       </c>
@@ -2641,7 +2641,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>195</v>
       </c>
@@ -2652,7 +2652,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>208</v>
       </c>
@@ -2663,7 +2663,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>211</v>
       </c>
@@ -2687,15 +2687,15 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="73.85546875" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="73.83203125" customWidth="1"/>
     <col min="3" max="3" width="73" customWidth="1"/>
-    <col min="4" max="4" width="59.7109375" customWidth="1"/>
+    <col min="4" max="4" width="59.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>191</v>
       </c>
@@ -2709,7 +2709,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>194</v>
       </c>
@@ -2721,7 +2721,7 @@
       </c>
       <c r="D2" s="2"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>203</v>
       </c>
@@ -2735,7 +2735,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>202</v>
       </c>
@@ -2756,30 +2756,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <dimension ref="A1:Q11"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="49.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="48.5703125" customWidth="1"/>
-    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.42578125" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="49.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="48.5" customWidth="1"/>
+    <col min="8" max="8" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="42.5" customWidth="1"/>
+    <col min="10" max="10" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.140625" customWidth="1"/>
+    <col min="12" max="12" width="11.1640625" customWidth="1"/>
     <col min="13" max="13" width="58" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="49" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="45.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="45.5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="24.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2832,7 +2832,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>68</v>
       </c>
@@ -2885,7 +2885,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>69</v>
       </c>
@@ -2938,7 +2938,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>61</v>
       </c>
@@ -2991,7 +2991,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>59</v>
       </c>
@@ -3044,7 +3044,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A6" s="17" t="s">
         <v>63</v>
       </c>
@@ -3097,7 +3097,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
         <v>119</v>
       </c>
@@ -3150,7 +3150,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A8" s="17" t="s">
         <v>64</v>
       </c>
@@ -3203,7 +3203,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A9" s="17" t="s">
         <v>66</v>
       </c>
@@ -3256,7 +3256,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A10" s="17" t="s">
         <v>47</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
         <v>101</v>
       </c>
@@ -3384,7 +3384,7 @@
       <selection activeCell="N34" sqref="N34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3396,15 +3396,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="86.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="59.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="26.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="86.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="59.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -3415,7 +3415,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>135</v>
       </c>
@@ -3424,7 +3424,7 @@
       </c>
       <c r="C2" s="5"/>
     </row>
-    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>57</v>
       </c>
@@ -3447,14 +3447,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.7109375" customWidth="1"/>
-    <col min="2" max="2" width="90.140625" customWidth="1"/>
-    <col min="3" max="3" width="108.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" customWidth="1"/>
+    <col min="2" max="2" width="90.1640625" customWidth="1"/>
+    <col min="3" max="3" width="108.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>56</v>
       </c>
@@ -3465,7 +3465,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>50</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>51</v>
       </c>
@@ -3487,7 +3487,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="28" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>53</v>
       </c>
@@ -3498,7 +3498,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>54</v>
       </c>
@@ -3509,7 +3509,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Change Excel file (email=False)
</commit_message>
<xml_diff>
--- a/runtime/apps/delphes/delphes.xlsx
+++ b/runtime/apps/delphes/delphes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime/apps/delphes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD3D71B-062A-8E46-B2A3-B1F4CC310781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B766DC7-10C7-E84D-8E64-902C995506F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="760" windowWidth="34680" windowHeight="15720" tabRatio="973" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="15720" tabRatio="973" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -1843,7 +1843,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1968,7 +1968,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2048,7 +2048,7 @@
         <v>189</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>188</v>
@@ -2757,7 +2757,7 @@
   <dimension ref="A1:Q11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Change Email distribution. New from address Athena.Delphes@gmail.com. Send Email to 2 addresses. Implement Bcc (not used for the moment)
</commit_message>
<xml_diff>
--- a/runtime/apps/delphes/delphes.xlsx
+++ b/runtime/apps/delphes/delphes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime/apps/delphes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD42177-F77B-8B4B-BBA3-A648475D10AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AAD38B7-0BF0-CF4F-BAEB-E7F69659B55E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="15720" tabRatio="973" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="305">
   <si>
     <t>Parameter</t>
   </si>
@@ -318,9 +318,6 @@
     <t>password</t>
   </si>
   <si>
-    <t>bceo rdxm suuv orul</t>
-  </si>
-  <si>
     <t>smtp.gmail.com</t>
   </si>
   <si>
@@ -337,12 +334,6 @@
   </si>
   <si>
     <t>agent_email_address</t>
-  </si>
-  <si>
-    <t>envoishibou78@gmail.com</t>
-  </si>
-  <si>
-    <t>pocagent78@gmail.com</t>
   </si>
   <si>
     <t>78235346097</t>
@@ -998,6 +989,18 @@
 Sans action dans les prochains jours, il risquera de perdre son travail.
 Je vous remercie par avance et vous prie de noter l'urgence. Il risque son emploi, c'est donc très important.
 Monsieur C aimerait, par ailleurs, faire une demande d'Asile à la France.</t>
+  </si>
+  <si>
+    <t>pref-delphes-sejour@yvelines.gouv.fr,pref-delphes-asile@yvelines.gouv.fr</t>
+  </si>
+  <si>
+    <t>Athena.Delphes@gmail.com</t>
+  </si>
+  <si>
+    <t>tubd yhuh fgiq hqrs</t>
+  </si>
+  <si>
+    <t>Would be better to separate separate asile/sejour</t>
   </si>
 </sst>
 </file>
@@ -1463,12 +1466,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1481,10 +1484,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>6</v>
@@ -1498,10 +1501,10 @@
         <v>43</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -1515,10 +1518,10 @@
         <v>44</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>9</v>
@@ -1529,13 +1532,13 @@
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -1549,10 +1552,10 @@
         <v>45</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
@@ -1566,10 +1569,10 @@
         <v>46</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -1580,13 +1583,13 @@
     </row>
     <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
@@ -1597,13 +1600,13 @@
     </row>
     <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
@@ -1614,13 +1617,13 @@
     </row>
     <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
@@ -1631,13 +1634,13 @@
     </row>
     <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>16</v>
@@ -1648,13 +1651,13 @@
     </row>
     <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>17</v>
@@ -1665,13 +1668,13 @@
     </row>
     <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>18</v>
@@ -1682,13 +1685,13 @@
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>19</v>
@@ -1699,13 +1702,13 @@
     </row>
     <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>20</v>
@@ -1716,13 +1719,13 @@
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>21</v>
@@ -1733,13 +1736,13 @@
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>22</v>
@@ -1750,13 +1753,13 @@
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>23</v>
@@ -1767,13 +1770,13 @@
     </row>
     <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>24</v>
@@ -1784,13 +1787,13 @@
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>25</v>
@@ -1801,19 +1804,19 @@
     </row>
     <row r="24" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
   </sheetData>
@@ -1861,79 +1864,79 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>259</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>261</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>264</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="18" t="s">
         <v>269</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C3" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D3" s="18" t="s">
-        <v>272</v>
-      </c>
       <c r="E3" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="18" t="s">
         <v>270</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>260</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>107</v>
-      </c>
-      <c r="D4" s="18" t="s">
-        <v>273</v>
-      </c>
       <c r="E4" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -1968,13 +1971,13 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="58.83203125" customWidth="1"/>
     <col min="3" max="3" width="70.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1991,25 +1994,27 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>302</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>94</v>
-      </c>
       <c r="B3" s="12" t="s">
-        <v>96</v>
-      </c>
-      <c r="C3" s="5"/>
+        <v>301</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>63</v>
@@ -2021,7 +2026,7 @@
         <v>86</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C5" s="5"/>
     </row>
@@ -2030,13 +2035,13 @@
         <v>87</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>88</v>
+        <v>303</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B7" s="5">
         <v>587</v>
@@ -2045,22 +2050,21 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{D837CF12-5C63-4697-8041-1E2C28E86DD4}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{4DA7E683-0DA1-40B9-9F1D-EC7A05076326}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{EA35456F-8910-A447-A530-A1B5920653C2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -2085,10 +2089,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C1" s="9" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>83</v>
@@ -2099,36 +2103,36 @@
     </row>
     <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>82</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2171,7 +2175,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2179,288 +2183,288 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="B9" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>280</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>280</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>282</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>279</v>
       </c>
-      <c r="B10" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>281</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>282</v>
-      </c>
       <c r="E10" s="7" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="B12" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>241</v>
-      </c>
-      <c r="D12" s="7" t="s">
-        <v>244</v>
-      </c>
       <c r="E12" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="B14" s="7" t="s">
+      <c r="C14" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="D14" s="7" t="s">
         <v>287</v>
       </c>
-      <c r="C14" s="7" t="s">
-        <v>287</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>290</v>
-      </c>
       <c r="E14" s="7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B15" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="C15" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>288</v>
-      </c>
-      <c r="C15" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="D15" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>289</v>
-      </c>
       <c r="C16" s="7" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
+        <v>289</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="D17" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>295</v>
-      </c>
-      <c r="D17" s="7" t="s">
-        <v>298</v>
-      </c>
       <c r="E17" s="7" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="B18" s="7" t="s">
         <v>293</v>
       </c>
-      <c r="B18" s="7" t="s">
+      <c r="C18" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>295</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>296</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>296</v>
-      </c>
-      <c r="D18" s="7" t="s">
-        <v>298</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>297</v>
-      </c>
       <c r="C19" s="7" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="E19" s="22" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -2499,19 +2503,19 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -2548,64 +2552,64 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -2632,46 +2636,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2697,53 +2701,53 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>206</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -2784,28 +2788,28 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>67</v>
@@ -2820,7 +2824,7 @@
         <v>72</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>7</v>
@@ -2837,52 +2841,52 @@
         <v>68</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="D2" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="H2" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="D2" s="7" t="s">
+      <c r="I2" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>111</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="F2" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="G2" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>113</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>114</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>85</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -2893,25 +2897,25 @@
         <v>4</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>70</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>71</v>
@@ -2920,22 +2924,22 @@
         <v>85</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="P3" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -2946,49 +2950,49 @@
         <v>4</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>62</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>79</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="P4" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -2999,49 +3003,49 @@
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>60</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>80</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="P5" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -3052,102 +3056,102 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>65</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J6" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="P6" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="P7" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -3158,49 +3162,49 @@
         <v>4</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="P8" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -3208,43 +3212,43 @@
         <v>66</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>107</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="H9" s="15" t="s">
         <v>110</v>
       </c>
-      <c r="C9" s="7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="E9" s="8" t="s">
-        <v>245</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>113</v>
-      </c>
       <c r="I9" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>43</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>48</v>
@@ -3253,7 +3257,7 @@
         <v>76</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -3264,40 +3268,40 @@
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F10" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G10" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H10" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I10" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="K10" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="L10" s="8" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="M10" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="O10" s="7" t="s">
         <v>42</v>
@@ -3306,60 +3310,60 @@
         <v>76</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="P11" s="7" t="s">
         <v>76</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
   </sheetData>
@@ -3417,10 +3421,10 @@
     </row>
     <row r="2" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -3429,7 +3433,7 @@
         <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -3459,7 +3463,7 @@
         <v>56</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>58</v>
@@ -3470,10 +3474,10 @@
         <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -3481,7 +3485,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>52</v>
@@ -3492,10 +3496,10 @@
         <v>53</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -3503,10 +3507,10 @@
         <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -3514,10 +3518,10 @@
         <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New email template for API expiration
</commit_message>
<xml_diff>
--- a/runtime/apps/delphes/delphes.xlsx
+++ b/runtime/apps/delphes/delphes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime/apps/delphes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD50317-DDBD-AA49-A07D-90B41C4098FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0D6FCD-BAF0-AB40-BAFA-198CC0678CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="15720" tabRatio="973" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="15720" tabRatio="973" firstSheet="2" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -345,10 +345,6 @@
     <t>distribution_engine</t>
   </si>
   <si>
-    <t>{prenom} {nom},
-Nous avons traité votre demande du {date_demande} en rapport avec l'expiration d'une API</t>
-  </si>
-  <si>
     <t>refugie_ou_protege_subsidiaire</t>
   </si>
   <si>
@@ -1001,6 +997,16 @@
   </si>
   <si>
     <t>Would be better to separate separate asile/sejour</t>
+  </si>
+  <si>
+    <t>Madame, Monsieur,
+Nous accusons réception de votre demande du {date_demande} concernant l’expiration de votre Autorisation Provisoire de Séjour (API).
+Après examen de votre dossier, nous vous informons que votre demande a été enregistrée et traitée par nos services. Votre situation a bien été prise en compte et les éléments transmis seront intégrés à votre dossier en cours.
+Conformément à la réglementation, vous serez prochainement contacté afin de finaliser la procédure (convocation en préfecture ou communication de la décision administrative). Dans l’attente, il est important de conserver les justificatifs de dépôt ou de renouvellement qui vous ont été remis. Ceux-ci tiennent lieu de preuve de la régularité de votre séjour jusqu’à la notification d’une décision officielle.
+Nous vous invitons à rester attentif aux communications de la préfecture et à consulter régulièrement vos courriels. Pour toute question complémentaire ou en cas de modification de votre situation personnelle, vous pouvez contacter le service des étrangers par courrier électronique à l’adresse suivante : [adresse générique du service] ou par téléphone aux horaires d’accueil indiqués sur notre site.
+Nous vous prions d’agréer, {prenom} {nom}, l’expression de notre considération distinguée.
+Direction des migrations et de l'intégration
+Préfecture des Yvelines</t>
   </si>
 </sst>
 </file>
@@ -1466,12 +1472,12 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -1484,10 +1490,10 @@
         <v>3</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>6</v>
@@ -1501,10 +1507,10 @@
         <v>43</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -1518,10 +1524,10 @@
         <v>44</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>9</v>
@@ -1532,13 +1538,13 @@
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -1552,10 +1558,10 @@
         <v>45</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
@@ -1569,10 +1575,10 @@
         <v>46</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -1583,13 +1589,13 @@
     </row>
     <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
@@ -1600,13 +1606,13 @@
     </row>
     <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
@@ -1617,13 +1623,13 @@
     </row>
     <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
@@ -1634,13 +1640,13 @@
     </row>
     <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>16</v>
@@ -1651,13 +1657,13 @@
     </row>
     <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>17</v>
@@ -1668,13 +1674,13 @@
     </row>
     <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>18</v>
@@ -1685,13 +1691,13 @@
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>19</v>
@@ -1702,13 +1708,13 @@
     </row>
     <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>20</v>
@@ -1719,13 +1725,13 @@
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>21</v>
@@ -1736,13 +1742,13 @@
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>22</v>
@@ -1753,13 +1759,13 @@
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>23</v>
@@ -1770,13 +1776,13 @@
     </row>
     <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>24</v>
@@ -1787,13 +1793,13 @@
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>25</v>
@@ -1804,19 +1810,19 @@
     </row>
     <row r="24" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
   </sheetData>
@@ -1864,79 +1870,79 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>258</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>259</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>260</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>261</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -1970,7 +1976,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -1997,7 +2003,7 @@
         <v>92</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -2006,10 +2012,10 @@
         <v>93</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2035,7 +2041,7 @@
         <v>87</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -2050,13 +2056,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -2072,8 +2078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2089,10 +2095,10 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>129</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>130</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>83</v>
@@ -2101,38 +2107,38 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="350" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>176</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>177</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>82</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>97</v>
+        <v>304</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="B3" s="5" t="s">
-        <v>178</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>179</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="2" t="s">
         <v>102</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -2175,7 +2181,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2183,288 +2189,288 @@
         <v>3</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>244</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B7" s="7" t="s">
         <v>124</v>
       </c>
-      <c r="B7" s="7" t="s">
-        <v>125</v>
-      </c>
       <c r="C7" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D8" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>278</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>279</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>280</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>236</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>238</v>
-      </c>
       <c r="C12" s="7" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>239</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>241</v>
-      </c>
       <c r="E13" s="7" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>287</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>287</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>286</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>286</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>287</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>295</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>295</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>293</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>294</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="22" t="s">
         <v>295</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -2503,19 +2509,19 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -2561,55 +2567,55 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -2636,46 +2642,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>192</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>194</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>193</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>206</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>209</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>210</v>
       </c>
     </row>
   </sheetData>
@@ -2701,53 +2707,53 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>190</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>196</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>197</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>203</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>204</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -2788,28 +2794,28 @@
         <v>3</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>67</v>
@@ -2824,7 +2830,7 @@
         <v>72</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>7</v>
@@ -2841,52 +2847,52 @@
         <v>68</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>108</v>
-      </c>
       <c r="E2" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H2" s="15" t="s">
+        <v>109</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="J2" s="8" t="s">
         <v>110</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="J2" s="8" t="s">
-        <v>111</v>
       </c>
       <c r="K2" s="8" t="s">
         <v>85</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -2897,25 +2903,25 @@
         <v>4</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>70</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>71</v>
@@ -2924,22 +2930,22 @@
         <v>85</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P3" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -2950,49 +2956,49 @@
         <v>4</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>62</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>79</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P4" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -3003,49 +3009,49 @@
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>60</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>80</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P5" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -3056,102 +3062,102 @@
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>65</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>90</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P6" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A7" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B7" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G7" s="16" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P7" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -3162,49 +3168,49 @@
         <v>4</v>
       </c>
       <c r="C8" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>141</v>
       </c>
-      <c r="D8" s="7" t="s">
-        <v>142</v>
-      </c>
       <c r="E8" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>94</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="P8" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -3212,43 +3218,43 @@
         <v>66</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="H9" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="E9" s="8" t="s">
-        <v>242</v>
-      </c>
-      <c r="F9" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>110</v>
-      </c>
       <c r="I9" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>43</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>48</v>
@@ -3257,7 +3263,7 @@
         <v>76</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -3268,40 +3274,40 @@
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>73</v>
       </c>
       <c r="E10" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>297</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>242</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>298</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>243</v>
-      </c>
       <c r="M10" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="O10" s="7" t="s">
         <v>42</v>
@@ -3310,60 +3316,60 @@
         <v>76</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A11" s="17" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" s="17" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="D11" s="7" t="s">
-        <v>147</v>
-      </c>
       <c r="E11" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O11" s="7" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="P11" s="7" t="s">
         <v>76</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -3421,10 +3427,10 @@
     </row>
     <row r="2" spans="1:3" ht="64" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -3433,7 +3439,7 @@
         <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -3463,7 +3469,7 @@
         <v>56</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>58</v>
@@ -3474,10 +3480,10 @@
         <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="48" x14ac:dyDescent="0.2">
@@ -3485,7 +3491,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>52</v>
@@ -3496,10 +3502,10 @@
         <v>53</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -3507,10 +3513,10 @@
         <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -3518,10 +3524,10 @@
         <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ignore log file, fix next config, display generated email with line breaks
</commit_message>
<xml_diff>
--- a/runtime/apps/delphes/delphes.xlsx
+++ b/runtime/apps/delphes/delphes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime/apps/delphes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB0D6FCD-BAF0-AB40-BAFA-198CC0678CB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DDF581-4E6A-3042-B901-C55093260E18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="15720" tabRatio="973" firstSheet="2" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -999,7 +999,7 @@
     <t>Would be better to separate separate asile/sejour</t>
   </si>
   <si>
-    <t>Madame, Monsieur,
+    <t>{prenom} {nom},
 Nous accusons réception de votre demande du {date_demande} concernant l’expiration de votre Autorisation Provisoire de Séjour (API).
 Après examen de votre dossier, nous vous informons que votre demande a été enregistrée et traitée par nos services. Votre situation a bien été prise en compte et les éléments transmis seront intégrés à votre dossier en cours.
 Conformément à la réglementation, vous serez prochainement contacté afin de finaliser la procédure (convocation en préfecture ou communication de la décision administrative). Dans l’attente, il est important de conserver les justificatifs de dépôt ou de renouvellement qui vous ont été remis. Ceux-ci tiennent lieu de preuve de la régularité de votre séjour jusqu’à la notification d’une décision officielle.
@@ -2079,7 +2079,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update Excel file for Delphes
</commit_message>
<xml_diff>
--- a/runtime/apps/delphes/delphes.xlsx
+++ b/runtime/apps/delphes/delphes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime/apps/delphes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23676309-9504-2940-BBE8-A92ED657E636}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6D2FB5-5C2B-D04E-A336-2C35E753E30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" tabRatio="973" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" tabRatio="973" firstSheet="2" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="610" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="359">
   <si>
     <t>Parameter</t>
   </si>
@@ -512,9 +512,6 @@
     <t xml:space="preserve">Attestation de Prolongation de l’Instruction, document généré depuis la plateforme ANEF </t>
   </si>
   <si>
-    <t>ATtestation de Demande d’Asile</t>
-  </si>
-  <si>
     <t>Document de Circulation pour Etranger Mineur</t>
   </si>
   <si>
@@ -1161,6 +1158,22 @@
   </si>
   <si>
     <t>L'API expirée depuis {0} jour(s)</t>
+  </si>
+  <si>
+    <t>atda</t>
+  </si>
+  <si>
+    <t>Votre ATDA</t>
+  </si>
+  <si>
+    <t>Attestation de Demande d’Asile</t>
+  </si>
+  <si>
+    <t>{prenom} {nom},
+Nous accusons réception de votre demande du {date_demande} concernant l'expiration de votre Attestation de Demande d’Asile (ATDA).
+Nous vous prions d’agréer, {prenom} {nom}, l’expression de notre considération distinguée.
+Direction des migrations et de l'intégration
+Préfecture des Yvelines</t>
   </si>
 </sst>
 </file>
@@ -1611,7 +1624,7 @@
   <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1661,10 +1674,10 @@
         <v>43</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>8</v>
@@ -1678,10 +1691,10 @@
         <v>44</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>9</v>
@@ -1692,13 +1705,13 @@
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>10</v>
@@ -1712,10 +1725,10 @@
         <v>45</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>11</v>
@@ -1729,10 +1742,10 @@
         <v>46</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -1743,13 +1756,13 @@
     </row>
     <row r="11" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>13</v>
@@ -1760,13 +1773,13 @@
     </row>
     <row r="12" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>14</v>
@@ -1777,13 +1790,13 @@
     </row>
     <row r="13" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>15</v>
@@ -1794,13 +1807,13 @@
     </row>
     <row r="14" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>16</v>
@@ -1811,13 +1824,13 @@
     </row>
     <row r="15" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>17</v>
@@ -1828,13 +1841,13 @@
     </row>
     <row r="16" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A16" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>18</v>
@@ -1845,13 +1858,13 @@
     </row>
     <row r="17" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>19</v>
@@ -1862,13 +1875,13 @@
     </row>
     <row r="18" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="5" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>20</v>
@@ -1879,13 +1892,13 @@
     </row>
     <row r="19" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>21</v>
@@ -1896,13 +1909,13 @@
     </row>
     <row r="20" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>22</v>
@@ -1913,13 +1926,13 @@
     </row>
     <row r="21" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A21" s="5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D21" s="2" t="s">
         <v>23</v>
@@ -1930,13 +1943,13 @@
     </row>
     <row r="22" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A22" s="5" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>24</v>
@@ -1947,13 +1960,13 @@
     </row>
     <row r="23" spans="1:5" ht="32" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>25</v>
@@ -1964,13 +1977,13 @@
     </row>
     <row r="24" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A24" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>26</v>
@@ -1981,6 +1994,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2006,7 +2020,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2024,79 +2038,79 @@
         <v>3</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C1" s="6" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>256</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>257</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>258</v>
-      </c>
-      <c r="F1" s="6" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E2" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C3" s="19" t="s">
         <v>103</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C4" s="19" t="s">
         <v>103</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>
@@ -2130,7 +2144,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AD020DE-44B7-44EF-BEA3-8491F2595E0A}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -2157,7 +2171,7 @@
         <v>92</v>
       </c>
       <c r="B2" s="12" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -2166,10 +2180,10 @@
         <v>93</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2195,7 +2209,7 @@
         <v>87</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C6" s="5"/>
     </row>
@@ -2210,13 +2224,13 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
   </sheetData>
@@ -2231,17 +2245,17 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="21.6640625" customWidth="1"/>
     <col min="3" max="3" width="101" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" customWidth="1"/>
+    <col min="4" max="4" width="25" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="101" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2267,16 +2281,16 @@
         <v>99</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>175</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>176</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>82</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="144" x14ac:dyDescent="0.2">
@@ -2284,10 +2298,10 @@
         <v>100</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>178</v>
       </c>
       <c r="D3" s="5" t="s">
         <v>101</v>
@@ -2296,8 +2310,22 @@
         <v>102</v>
       </c>
     </row>
+    <row r="4" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>358</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -2346,282 +2374,282 @@
         <v>6</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>242</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B7" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E10" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D13" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>352</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="C17" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="C17" s="7" t="s">
-        <v>354</v>
-      </c>
       <c r="D17" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2648,7 +2676,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
@@ -2662,10 +2690,10 @@
         <v>6</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>241</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>242</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -2679,10 +2707,10 @@
         <v>117</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -2696,10 +2724,10 @@
         <v>118</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -2713,10 +2741,10 @@
         <v>119</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -2730,214 +2758,214 @@
         <v>124</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D8" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E8" s="7" t="s">
         <v>277</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D9" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E9" s="7" t="s">
         <v>277</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B10" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="D10" s="7" t="s">
         <v>276</v>
       </c>
-      <c r="C10" s="7" t="s">
-        <v>276</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="7" t="s">
         <v>277</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>233</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>234</v>
-      </c>
       <c r="C11" s="7" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
+        <v>234</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>235</v>
       </c>
-      <c r="B12" s="7" t="s">
-        <v>236</v>
-      </c>
       <c r="C12" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="B13" s="7" t="s">
+      <c r="C13" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="D13" s="7" t="s">
         <v>238</v>
       </c>
-      <c r="C13" s="7" t="s">
-        <v>238</v>
-      </c>
-      <c r="D13" s="7" t="s">
-        <v>239</v>
-      </c>
       <c r="E13" s="7" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>285</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>285</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B16" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D16" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>284</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="E16" s="7" t="s">
         <v>285</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>293</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>293</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B19" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>292</v>
       </c>
-      <c r="C19" s="7" t="s">
-        <v>292</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="22" t="s">
         <v>293</v>
-      </c>
-      <c r="E19" s="22" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -2977,19 +3005,19 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -3002,7 +3030,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{549C78AA-1218-455B-9887-3E0A5E59C6C7}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
@@ -3035,55 +3063,55 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C4" s="5"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" ht="48" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C6" s="5"/>
     </row>
     <row r="7" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:3" ht="240" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C8" s="5"/>
     </row>
@@ -3110,46 +3138,46 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>191</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>193</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>205</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>207</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>208</v>
       </c>
     </row>
   </sheetData>
@@ -3175,53 +3203,53 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="C1" s="4" t="s">
-        <v>189</v>
-      </c>
       <c r="D1" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>195</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>196</v>
       </c>
       <c r="D2" s="2"/>
     </row>
     <row r="3" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>202</v>
       </c>
-      <c r="C3" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D4" s="2"/>
     </row>
@@ -3234,7 +3262,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
   <dimension ref="A1:Q12"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
@@ -3283,7 +3311,7 @@
         <v>105</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="J1" s="4" t="s">
         <v>67</v>
@@ -3324,19 +3352,19 @@
         <v>107</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H2" s="15" t="s">
         <v>109</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J2" s="8" t="s">
         <v>110</v>
@@ -3345,22 +3373,22 @@
         <v>85</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M2" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N2" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="O2" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P2" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q2" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -3377,19 +3405,19 @@
         <v>70</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I3" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J3" s="8" t="s">
         <v>71</v>
@@ -3398,22 +3426,22 @@
         <v>85</v>
       </c>
       <c r="L3" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N3" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="O3" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P3" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q3" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -3430,43 +3458,43 @@
         <v>62</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H4" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I4" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J4" s="8" t="s">
         <v>79</v>
       </c>
       <c r="K4" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L4" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N4" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="O4" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P4" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q4" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
@@ -3483,43 +3511,43 @@
         <v>60</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G5" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I5" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J5" s="8" t="s">
         <v>80</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M5" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N5" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="O5" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P5" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q5" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
@@ -3536,43 +3564,43 @@
         <v>65</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>114</v>
       </c>
       <c r="H6" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>90</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N6" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="O6" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P6" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q6" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
@@ -3589,7 +3617,7 @@
         <v>147</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F7" s="16" t="s">
         <v>116</v>
@@ -3598,34 +3626,34 @@
         <v>116</v>
       </c>
       <c r="H7" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I7" s="7" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J7" s="8" t="s">
         <v>120</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M7" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N7" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="O7" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P7" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q7" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
@@ -3642,7 +3670,7 @@
         <v>141</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F8" s="15" t="s">
         <v>113</v>
@@ -3651,34 +3679,34 @@
         <v>113</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J8" s="8" t="s">
         <v>94</v>
       </c>
       <c r="K8" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L8" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M8" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N8" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="O8" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P8" s="7" t="s">
         <v>75</v>
       </c>
       <c r="Q8" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
@@ -3695,34 +3723,34 @@
         <v>108</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G9" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H9" s="15" t="s">
         <v>109</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J9" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K9" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L9" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M9" s="5" t="s">
         <v>43</v>
       </c>
       <c r="N9" s="7" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="O9" s="7" t="s">
         <v>48</v>
@@ -3731,7 +3759,7 @@
         <v>76</v>
       </c>
       <c r="Q9" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
@@ -3748,34 +3776,34 @@
         <v>73</v>
       </c>
       <c r="E10" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="I10" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="L10" s="8" t="s">
         <v>240</v>
       </c>
-      <c r="F10" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="G10" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="J10" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>296</v>
-      </c>
-      <c r="L10" s="8" t="s">
-        <v>241</v>
-      </c>
       <c r="M10" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N10" s="7" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="O10" s="7" t="s">
         <v>42</v>
@@ -3784,7 +3812,7 @@
         <v>76</v>
       </c>
       <c r="Q10" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
@@ -3801,34 +3829,34 @@
         <v>146</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="G11" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="J11" s="14" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="K11" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M11" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="N11" s="7" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="O11" s="7" t="s">
         <v>98</v>
@@ -3837,60 +3865,60 @@
         <v>76</v>
       </c>
       <c r="Q11" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A12" s="17" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B12" s="17" t="s">
         <v>4</v>
       </c>
       <c r="C12" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="D12" s="7" t="s">
         <v>305</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>247</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>350</v>
+      </c>
+      <c r="J12" s="14" t="s">
         <v>306</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>240</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>248</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>351</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>307</v>
-      </c>
       <c r="K12" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="L12" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M12" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N12" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="O12" s="8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="P12" s="7" t="s">
         <v>76</v>
       </c>
       <c r="Q12" s="8" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -3925,7 +3953,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -3951,7 +3981,7 @@
         <v>131</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C2" s="5"/>
     </row>
@@ -3960,7 +3990,7 @@
         <v>57</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C3" s="5"/>
     </row>
@@ -3975,7 +4005,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4001,7 +4031,7 @@
         <v>50</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>148</v>
@@ -4012,7 +4042,7 @@
         <v>51</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>52</v>
@@ -4023,7 +4053,7 @@
         <v>53</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>149</v>
@@ -4034,10 +4064,10 @@
         <v>54</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>150</v>
+        <v>357</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -4045,10 +4075,10 @@
         <v>55</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add runtime_dev, fix main.py, accept --reload for launcher_api.py
</commit_message>
<xml_diff>
--- a/runtime/apps/delphes/delphes.xlsx
+++ b/runtime/apps/delphes/delphes.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11012"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime/apps/delphes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF6D2FB5-5C2B-D04E-A336-2C35E753E30B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F946D58D-4AAB-6E45-B035-6A3822EB5A7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19920" tabRatio="973" firstSheet="2" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="3" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="359">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="615" uniqueCount="361">
   <si>
     <t>Parameter</t>
   </si>
@@ -1174,6 +1174,16 @@
 Nous vous prions d’agréer, {prenom} {nom}, l’expression de notre considération distinguée.
 Direction des migrations et de l'intégration
 Préfecture des Yvelines</t>
+  </si>
+  <si>
+    <t>Your request related to your ATDA</t>
+  </si>
+  <si>
+    <t>{prenom} {nom},
+We acknowledge receipt of your request dated {date_request} concerning the expiration of your Certificate of Asylum Application (ATDA).
+Yours sincerely,
+Migration and Integration Department
+Yvelines Prefecture</t>
   </si>
 </sst>
 </file>
@@ -2247,8 +2257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2314,8 +2324,12 @@
       <c r="A4" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+      <c r="B4" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>360</v>
+      </c>
       <c r="D4" s="5" t="s">
         <v>356</v>
       </c>

</xml_diff>

<commit_message>
Delphes new frontend first page, modif as per meeting with business
</commit_message>
<xml_diff>
--- a/runtime/apps/delphes/delphes.xlsx
+++ b/runtime/apps/delphes/delphes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joel/Documents/Dev/Athena/trusted-service/runtime/apps/delphes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F50D3D1-190C-DF44-8C17-E49E11475066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{184C58CD-2737-884C-8FE8-5ABFE174C630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="1" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="18860" tabRatio="973" firstSheet="4" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="APP &amp; MODEL" sheetId="25" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="749" uniqueCount="460">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="763" uniqueCount="463">
   <si>
     <t>Parameter</t>
   </si>
@@ -960,359 +960,508 @@
     <t>tubd yhuh fgiq hqrs</t>
   </si>
   <si>
+    <t>statut</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Statut</t>
+  </si>
+  <si>
+    <t>régulier</t>
+  </si>
+  <si>
+    <t>irrégulier</t>
+  </si>
+  <si>
+    <t>étudiant</t>
+  </si>
+  <si>
+    <t>visiteur</t>
+  </si>
+  <si>
+    <t>réfugié</t>
+  </si>
+  <si>
+    <t>protégé_subsidiaire</t>
+  </si>
+  <si>
+    <t>apatride</t>
+  </si>
+  <si>
+    <t>première_demande</t>
+  </si>
+  <si>
+    <t>renouvellement</t>
+  </si>
+  <si>
+    <t>citoyen_UE</t>
+  </si>
+  <si>
+    <t>conjoint_de_français</t>
+  </si>
+  <si>
+    <t>parent_d_enfant_français_mineur</t>
+  </si>
+  <si>
+    <t>passeport_talent</t>
+  </si>
+  <si>
+    <t>entrepreneur</t>
+  </si>
+  <si>
+    <t>vls_ts</t>
+  </si>
+  <si>
+    <t>En situation régulière</t>
+  </si>
+  <si>
+    <t>In a regular situation</t>
+  </si>
+  <si>
+    <t>In an irregular situation</t>
+  </si>
+  <si>
+    <t>Visteur</t>
+  </si>
+  <si>
+    <t>Visitor</t>
+  </si>
+  <si>
+    <t>Etudiant</t>
+  </si>
+  <si>
+    <t>Student</t>
+  </si>
+  <si>
+    <t>Première demande</t>
+  </si>
+  <si>
+    <t>First request</t>
+  </si>
+  <si>
+    <t>Visa long séjour valant titre de séjour</t>
+  </si>
+  <si>
+    <t>Long-stay visa equivalent to a residence permit</t>
+  </si>
+  <si>
+    <t>Renouvellement</t>
+  </si>
+  <si>
+    <t>Renewal</t>
+  </si>
+  <si>
+    <t>Citoyen de l'Union Européenne</t>
+  </si>
+  <si>
+    <t>Citizen of the European Union</t>
+  </si>
+  <si>
+    <t>Régugié</t>
+  </si>
+  <si>
+    <t>Refugee</t>
+  </si>
+  <si>
+    <t>Protégé subsidiaire</t>
+  </si>
+  <si>
+    <t>Subsidiary protection</t>
+  </si>
+  <si>
+    <t>Apatride</t>
+  </si>
+  <si>
+    <t>Conjoint de français</t>
+  </si>
+  <si>
+    <t>Parent d'enfant français mineur</t>
+  </si>
+  <si>
+    <t>Passeport Talent</t>
+  </si>
+  <si>
+    <t>Entrepreneur</t>
+  </si>
+  <si>
+    <t>Business owner</t>
+  </si>
+  <si>
+    <t>Talent Passport</t>
+  </si>
+  <si>
+    <t>Parent of a minor French child</t>
+  </si>
+  <si>
+    <t>Spouse of a French citizen</t>
+  </si>
+  <si>
+    <t>statuts</t>
+  </si>
+  <si>
+    <t>ne_sait_pas</t>
+  </si>
+  <si>
+    <t>I don't know</t>
+  </si>
+  <si>
+    <t>Je ne sais pas</t>
+  </si>
+  <si>
+    <t>atda</t>
+  </si>
+  <si>
+    <t>Votre ATDA</t>
+  </si>
+  <si>
+    <t>Attestation de Demande d’Asile</t>
+  </si>
+  <si>
+    <t>Your request related to your ATDA</t>
+  </si>
+  <si>
+    <t>{prenom} {nom},
+We acknowledge receipt of your request dated {date_request} concerning the expiration of your Certificate of Asylum Application (ATDA).
+Yours sincerely,
+Migration and Integration Department
+Yvelines Prefecture</t>
+  </si>
+  <si>
+    <t>difficulte_prise_rdv</t>
+  </si>
+  <si>
+    <t>DIFFICULTE DE PRISE DE RENDEZ-VOUS</t>
+  </si>
+  <si>
+    <t>Le demandeur exprime une difficulté à prendre un rendez-vous par quelque moyen que ce soit et pour quelque raison que ce soit</t>
+  </si>
+  <si>
+    <t>rdv_remise_de_titre</t>
+  </si>
+  <si>
+    <t>rdv_renouvellement_recepisse</t>
+  </si>
+  <si>
+    <t>rdv_renouvellement_titre_sejour_hors_anef</t>
+  </si>
+  <si>
+    <t>rdv_sauf_conduit</t>
+  </si>
+  <si>
+    <t>rdv_premiere_demande_titre_sejour</t>
+  </si>
+  <si>
+    <t>DIFFICULTY IN MAKING APPOINTMENTS</t>
+  </si>
+  <si>
+    <t>The applicant expresses difficulty in making an appointment by any means and for any reason.</t>
+  </si>
+  <si>
+    <t>MAKING AN APPOINTMENT DELIVERY OF DOCUMENTS</t>
+  </si>
+  <si>
+    <t>The applicant requests an appointment for the transfer of title.</t>
+  </si>
+  <si>
+    <t>MAKE AN APPOINTMENT RENEWAL RECEIPT</t>
+  </si>
+  <si>
+    <t>The applicant requests an appointment to renew their receipt.</t>
+  </si>
+  <si>
+    <t>MAKING AN APPOINTMENT TO RENEW YOUR RESIDENCE PERMIT OUTSIDE THE ANEF</t>
+  </si>
+  <si>
+    <t>The applicant requests an appointment to renew a residence permit. Their application is part of a process managed outside the ANEF website.</t>
+  </si>
+  <si>
+    <t>MAKING AN APPOINTMENT SAFE CONDUCT</t>
+  </si>
+  <si>
+    <t>The applicant requests an appointment for a safe conduct pass.</t>
+  </si>
+  <si>
+    <t>MAKING AN APPOINTMENT FIRST APPLICATION FOR A RESIDENCE PERMIT</t>
+  </si>
+  <si>
+    <t>motif_deces</t>
+  </si>
+  <si>
+    <t>Demande de sauf-conduit pour motif de décès</t>
+  </si>
+  <si>
+    <t>Request for safe passage due to death</t>
+  </si>
+  <si>
+    <t>Safe conduct is requested on grounds of death.</t>
+  </si>
+  <si>
+    <t>ACCUEIL</t>
+  </si>
+  <si>
+    <t>Veuillez vous présenter à l'accueil de la préfecture pour effectuer cette demande sur place.</t>
+  </si>
+  <si>
+    <t>Votre demande a été prise en compte. Un agent la traitera dans les plus brefs délais.</t>
+  </si>
+  <si>
+    <t>Your request has been registered. It will be processed by an agent.</t>
+  </si>
+  <si>
+    <t>Please visit [{0}]({1}).</t>
+  </si>
+  <si>
+    <t>Veuillez consulter la page [{0}]({1}).</t>
+  </si>
+  <si>
+    <t>Please go to the reception desk at the prefecture to make this request in person.</t>
+  </si>
+  <si>
+    <t>date_expiration_recepisse</t>
+  </si>
+  <si>
+    <t>Acknowledgement document expiry date (DD/MM/YYYY)</t>
+  </si>
+  <si>
+    <t>Date d'expiration du récépissé au format JJ/MM/AAAA</t>
+  </si>
+  <si>
+    <t>Acknowledgement document expiration date formatted as DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>date d'expiration du récépissé au format JJ/MM/AAAA</t>
+  </si>
+  <si>
+    <t>date_expiration_titre_sejour</t>
+  </si>
+  <si>
+    <t>Resident permit expiry date (DD/MM/YYYY)</t>
+  </si>
+  <si>
+    <t>Date d'expiration du titre de séjour au format JJ/MM/AAAA</t>
+  </si>
+  <si>
+    <t>Resident permit expiration date formatted as DD/MM/YYYY</t>
+  </si>
+  <si>
+    <t>date d'expiration du titre de séjour au format JJ/MM/AAAA</t>
+  </si>
+  <si>
+    <t>PRISE DE RENDEZ-VOUS PREMIERE DEMANDE DE TITRE DE SEJOUR</t>
+  </si>
+  <si>
+    <t>PRISE DE RENDEZ-VOUS SAUF-CONDUITS</t>
+  </si>
+  <si>
+    <t>PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF</t>
+  </si>
+  <si>
+    <t>PRISE DE RENDEZ-VOUS RENOUVELLEMENT RECEPISSE</t>
+  </si>
+  <si>
+    <t>PRISE DE RENDEZ-VOUS REMISE DE TITRES</t>
+  </si>
+  <si>
+    <t>Le demandeur désire prendre un rendez-vous. La raison du rendez-vous est : remise de titre</t>
+  </si>
+  <si>
+    <t>Le demandeur sollicite la prise d'un rendez-vous pour le renouvellement de son récépissé</t>
+  </si>
+  <si>
+    <t>Le demandeur demande à prendre un rendez-vous pour le renouvellement d'un titre de séjour. Sa demande s'inscrit dans un processus géré en dehors du site de l'anef</t>
+  </si>
+  <si>
+    <t>Le demandeur demande à prendre un rendez-vous pour un sauf-conduit</t>
+  </si>
+  <si>
+    <t>Le demandeur demande à prendre un rendez-vous pour une première demande de titre de séjour</t>
+  </si>
+  <si>
+    <t>dublin</t>
+  </si>
+  <si>
+    <t>Your request related to your Dublin procedure</t>
+  </si>
+  <si>
+    <t>{prenom} {nom},
+We acknowledge receipt of your request dated {date_request} concerning your Dublin procedure.
+Yours sincerely,
+Migration and Integration Department
+Yvelines Prefecture</t>
+  </si>
+  <si>
+    <t>Procédure Dublin en cours</t>
+  </si>
+  <si>
+    <t>asile_hebergement_urgence</t>
+  </si>
+  <si>
+    <t>aide_financiere_demandeur_asile</t>
+  </si>
+  <si>
+    <t>The applicant requests an appointment to submit an initial application for a residence permit.</t>
+  </si>
+  <si>
+    <t>The applicant wishes to return to their country for exceptional reasons (e.g. death of a relative, marriage of a relative, birth).</t>
+  </si>
+  <si>
+    <t>The applicant states that he wishes to apply for asylum.</t>
+  </si>
+  <si>
+    <t>DEMANDE D'AIDE FINANCIERE POUR UN DEMANDEUR D'ASILE</t>
+  </si>
+  <si>
+    <t>DEMANDE D'HEBERGEMENT D'URGENCE POUR UN DEMANDEUR D'ASILE</t>
+  </si>
+  <si>
+    <t>Le demandeur d'asile a besoin d'un hébergement d'urgence et en fait la demande</t>
+  </si>
+  <si>
+    <t>Le demandeur d'asile a besoin d'une aide financière et en fait la demande</t>
+  </si>
+  <si>
+    <t>APPLICATION FOR EMERGENCY ACCOMMODATION FOR AN ASYLUM SEEKER</t>
+  </si>
+  <si>
+    <t>APPLICATION FOR FINANCIAL ASSISTANCE FOR AN ASYLUM SEEKER</t>
+  </si>
+  <si>
+    <t>The asylum seeker requires emergency accommodation and has applied for it.</t>
+  </si>
+  <si>
+    <t>The asylum seeker requires financial assistance and is applying for it.</t>
+  </si>
+  <si>
+    <t>demandeur_d_asile</t>
+  </si>
+  <si>
+    <t>Demandeur d'asile</t>
+  </si>
+  <si>
+    <t>Asylum seeker</t>
+  </si>
+  <si>
+    <t>Le sauf-conduit est demandé pour motif de décès</t>
+  </si>
+  <si>
+    <t>demandeur d'asile</t>
+  </si>
+  <si>
+    <t>asylum seeker</t>
+  </si>
+  <si>
+    <t>aide_financiere_demandeur_asile asile_hebergement_urgence</t>
+  </si>
+  <si>
+    <t>RECEPISSE_VA_EXPIRER_DANS_X_JOURS</t>
+  </si>
+  <si>
+    <t>TITRE_SEJOUR_EXPIRE_DEPUIS_X_JOURS</t>
+  </si>
+  <si>
+    <t>TITRE_SEJOUR_VA_EXPIRER_DANS_X_JOURS</t>
+  </si>
+  <si>
+    <t>RELEVE_DE_L_ANEF</t>
+  </si>
+  <si>
+    <t>Please reach out to your contact at OFPRA or visit the[OFPRA website](https://www.usager.ofpra.gouv.fr/).</t>
+  </si>
+  <si>
+    <t>Veuillez vous adresser à votre contact OFPRA ou rendez-vous sur le site de l'[OFPRA](https://www.usager.ofpra.gouv.fr/).</t>
+  </si>
+  <si>
+    <t>Le récépissé va expirer dans {0} jour(s)</t>
+  </si>
+  <si>
+    <t>Le titre de séjour va expirer dans {0} jour(s)</t>
+  </si>
+  <si>
+    <t>Le titre de séjour est expiré depuis {0} jour(s)</t>
+  </si>
+  <si>
+    <t>L'API est expirée depuis {0} jour(s)</t>
+  </si>
+  <si>
+    <t>The receipt will expire in {0} day(s)</t>
+  </si>
+  <si>
+    <t>The residence permit will expire in {0} day(s)</t>
+  </si>
+  <si>
+    <t>The residence permit expired {0} day(s) ago</t>
+  </si>
+  <si>
+    <t>Relève de l'ANEF</t>
+  </si>
+  <si>
+    <t>Reports to ANEF</t>
+  </si>
+  <si>
+    <t>DEMANDEUR_D_ASILE</t>
+  </si>
+  <si>
+    <t>Est demadeur d'asile</t>
+  </si>
+  <si>
+    <t>Is an asylum seeker</t>
+  </si>
+  <si>
+    <t>STATUT</t>
+  </si>
+  <si>
+    <t>A déclaré le statut : {0}</t>
+  </si>
+  <si>
+    <t>Status is {0}</t>
+  </si>
+  <si>
+    <t>Si vous êtes sans solution, appeler le 115 pour trouver un hébergement d'urgence (appel gratuit).</t>
+  </si>
+  <si>
+    <t>If you are unable to find a solution, call 115 to find emergency accommodation (free call).</t>
+  </si>
+  <si>
+    <t>APPEL_115</t>
+  </si>
+  <si>
+    <t>AUCUNE_SOLUTION</t>
+  </si>
+  <si>
+    <t>La préfecture n'a aucune solution à vous proposer et nous en sommes désolés.</t>
+  </si>
+  <si>
+    <t>The prefecture has no solution to offer you, and we are sorry about that.</t>
+  </si>
+  <si>
+    <t>DEMANDE DE DUPLICATA</t>
+  </si>
+  <si>
+    <t>Le demandeur a besoin d'un duplicata</t>
+  </si>
+  <si>
+    <t>REQUEST FOR DUPLICATE</t>
+  </si>
+  <si>
+    <t>The applicant requires a duplicate copy.</t>
+  </si>
+  <si>
+    <t>duplicata</t>
+  </si>
+  <si>
+    <t>En situation irrégulière (sans titre de séjour valable)</t>
+  </si>
+  <si>
     <t>{prenom} {nom},
 Nous accusons réception de votre demande du {date_demande} concernant l’expiration de votre Autorisation Provisoire de Séjour (API).
 Après examen de votre dossier, nous vous informons que votre demande a été enregistrée et traitée par nos services. Votre situation a bien été prise en compte et les éléments transmis seront intégrés à votre dossier en cours.
 Conformément à la réglementation, vous serez prochainement contacté afin de finaliser la procédure (convocation en préfecture ou communication de la décision administrative). Dans l’attente, il est important de conserver les justificatifs de dépôt ou de renouvellement qui vous ont été remis. Ceux-ci tiennent lieu de preuve de la régularité de votre séjour jusqu’à la notification d’une décision officielle.
 Nous vous invitons à rester attentif aux communications de la préfecture et à consulter régulièrement vos courriels. Pour toute question complémentaire ou en cas de modification de votre situation personnelle, vous pouvez contacter le service des étrangers par courrier électronique à l’adresse suivante : [adresse générique du service] ou par téléphone aux horaires d’accueil indiqués sur notre site.
 Nous vous prions d’agréer, {prenom} {nom}, l’expression de notre considération distinguée.
-Direction des migrations et de l'intégration
-Préfecture des Yvelines</t>
-  </si>
-  <si>
-    <t>statut</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>Statut</t>
-  </si>
-  <si>
-    <t>régulier</t>
-  </si>
-  <si>
-    <t>irrégulier</t>
-  </si>
-  <si>
-    <t>étudiant</t>
-  </si>
-  <si>
-    <t>visiteur</t>
-  </si>
-  <si>
-    <t>réfugié</t>
-  </si>
-  <si>
-    <t>protégé_subsidiaire</t>
-  </si>
-  <si>
-    <t>apatride</t>
-  </si>
-  <si>
-    <t>première_demande</t>
-  </si>
-  <si>
-    <t>renouvellement</t>
-  </si>
-  <si>
-    <t>citoyen_UE</t>
-  </si>
-  <si>
-    <t>conjoint_de_français</t>
-  </si>
-  <si>
-    <t>parent_d_enfant_français_mineur</t>
-  </si>
-  <si>
-    <t>passeport_talent</t>
-  </si>
-  <si>
-    <t>entrepreneur</t>
-  </si>
-  <si>
-    <t>vls_ts</t>
-  </si>
-  <si>
-    <t>En situation régulière</t>
-  </si>
-  <si>
-    <t>En situation irrégulière</t>
-  </si>
-  <si>
-    <t>In a regular situation</t>
-  </si>
-  <si>
-    <t>In an irregular situation</t>
-  </si>
-  <si>
-    <t>Visteur</t>
-  </si>
-  <si>
-    <t>Visitor</t>
-  </si>
-  <si>
-    <t>Etudiant</t>
-  </si>
-  <si>
-    <t>Student</t>
-  </si>
-  <si>
-    <t>Première demande</t>
-  </si>
-  <si>
-    <t>First request</t>
-  </si>
-  <si>
-    <t>Visa long séjour valant titre de séjour</t>
-  </si>
-  <si>
-    <t>Long-stay visa equivalent to a residence permit</t>
-  </si>
-  <si>
-    <t>Renouvellement</t>
-  </si>
-  <si>
-    <t>Renewal</t>
-  </si>
-  <si>
-    <t>Citoyen de l'Union Européenne</t>
-  </si>
-  <si>
-    <t>Citizen of the European Union</t>
-  </si>
-  <si>
-    <t>Régugié</t>
-  </si>
-  <si>
-    <t>Refugee</t>
-  </si>
-  <si>
-    <t>Protégé subsidiaire</t>
-  </si>
-  <si>
-    <t>Subsidiary protection</t>
-  </si>
-  <si>
-    <t>Apatride</t>
-  </si>
-  <si>
-    <t>Conjoint de français</t>
-  </si>
-  <si>
-    <t>Parent d'enfant français mineur</t>
-  </si>
-  <si>
-    <t>Passeport Talent</t>
-  </si>
-  <si>
-    <t>Entrepreneur</t>
-  </si>
-  <si>
-    <t>Business owner</t>
-  </si>
-  <si>
-    <t>Talent Passport</t>
-  </si>
-  <si>
-    <t>Parent of a minor French child</t>
-  </si>
-  <si>
-    <t>Spouse of a French citizen</t>
-  </si>
-  <si>
-    <t>statuts</t>
-  </si>
-  <si>
-    <t>ne_sait_pas</t>
-  </si>
-  <si>
-    <t>I don't know</t>
-  </si>
-  <si>
-    <t>Je ne sais pas</t>
-  </si>
-  <si>
-    <t>atda</t>
-  </si>
-  <si>
-    <t>Votre ATDA</t>
-  </si>
-  <si>
-    <t>Attestation de Demande d’Asile</t>
-  </si>
-  <si>
-    <t>{prenom} {nom},
-Nous accusons réception de votre demande du {date_demande} concernant l'expiration de votre Attestation de Demande d’Asile (ATDA).
-Nous vous prions d’agréer, {prenom} {nom}, l’expression de notre considération distinguée.
-Direction des migrations et de l'intégration
-Préfecture des Yvelines</t>
-  </si>
-  <si>
-    <t>Your request related to your ATDA</t>
-  </si>
-  <si>
-    <t>{prenom} {nom},
-We acknowledge receipt of your request dated {date_request} concerning the expiration of your Certificate of Asylum Application (ATDA).
-Yours sincerely,
-Migration and Integration Department
-Yvelines Prefecture</t>
-  </si>
-  <si>
-    <t>difficulte_prise_rdv</t>
-  </si>
-  <si>
-    <t>DIFFICULTE DE PRISE DE RENDEZ-VOUS</t>
-  </si>
-  <si>
-    <t>Le demandeur exprime une difficulté à prendre un rendez-vous par quelque moyen que ce soit et pour quelque raison que ce soit</t>
-  </si>
-  <si>
-    <t>rdv_remise_de_titre</t>
-  </si>
-  <si>
-    <t>rdv_renouvellement_recepisse</t>
-  </si>
-  <si>
-    <t>rdv_renouvellement_titre_sejour_hors_anef</t>
-  </si>
-  <si>
-    <t>rdv_sauf_conduit</t>
-  </si>
-  <si>
-    <t>rdv_premiere_demande_titre_sejour</t>
-  </si>
-  <si>
-    <t>DIFFICULTY IN MAKING APPOINTMENTS</t>
-  </si>
-  <si>
-    <t>The applicant expresses difficulty in making an appointment by any means and for any reason.</t>
-  </si>
-  <si>
-    <t>MAKING AN APPOINTMENT DELIVERY OF DOCUMENTS</t>
-  </si>
-  <si>
-    <t>The applicant requests an appointment for the transfer of title.</t>
-  </si>
-  <si>
-    <t>MAKE AN APPOINTMENT RENEWAL RECEIPT</t>
-  </si>
-  <si>
-    <t>The applicant requests an appointment to renew their receipt.</t>
-  </si>
-  <si>
-    <t>MAKING AN APPOINTMENT TO RENEW YOUR RESIDENCE PERMIT OUTSIDE THE ANEF</t>
-  </si>
-  <si>
-    <t>The applicant requests an appointment to renew a residence permit. Their application is part of a process managed outside the ANEF website.</t>
-  </si>
-  <si>
-    <t>MAKING AN APPOINTMENT SAFE CONDUCT</t>
-  </si>
-  <si>
-    <t>The applicant requests an appointment for a safe conduct pass.</t>
-  </si>
-  <si>
-    <t>MAKING AN APPOINTMENT FIRST APPLICATION FOR A RESIDENCE PERMIT</t>
-  </si>
-  <si>
-    <t>motif_deces</t>
-  </si>
-  <si>
-    <t>Demande de sauf-conduit pour motif de décès</t>
-  </si>
-  <si>
-    <t>Request for safe passage due to death</t>
-  </si>
-  <si>
-    <t>Safe conduct is requested on grounds of death.</t>
-  </si>
-  <si>
-    <t>ACCUEIL</t>
-  </si>
-  <si>
-    <t>Veuillez vous présenter à l'accueil de la préfecture pour effectuer cette demande sur place.</t>
-  </si>
-  <si>
-    <t>Votre demande a été prise en compte. Un agent la traitera dans les plus brefs délais.</t>
-  </si>
-  <si>
-    <t>Your request has been registered. It will be processed by an agent.</t>
-  </si>
-  <si>
-    <t>Please visit [{0}]({1}).</t>
-  </si>
-  <si>
-    <t>Veuillez consulter la page [{0}]({1}).</t>
-  </si>
-  <si>
-    <t>Please go to the reception desk at the prefecture to make this request in person.</t>
-  </si>
-  <si>
-    <t>date_expiration_recepisse</t>
-  </si>
-  <si>
-    <t>Acknowledgement document expiry date (DD/MM/YYYY)</t>
-  </si>
-  <si>
-    <t>Date d'expiration du récépissé au format JJ/MM/AAAA</t>
-  </si>
-  <si>
-    <t>Acknowledgement document expiration date formatted as DD/MM/YYYY</t>
-  </si>
-  <si>
-    <t>date d'expiration du récépissé au format JJ/MM/AAAA</t>
-  </si>
-  <si>
-    <t>date_expiration_titre_sejour</t>
-  </si>
-  <si>
-    <t>Resident permit expiry date (DD/MM/YYYY)</t>
-  </si>
-  <si>
-    <t>Date d'expiration du titre de séjour au format JJ/MM/AAAA</t>
-  </si>
-  <si>
-    <t>Resident permit expiration date formatted as DD/MM/YYYY</t>
-  </si>
-  <si>
-    <t>date d'expiration du titre de séjour au format JJ/MM/AAAA</t>
-  </si>
-  <si>
-    <t>PRISE DE RENDEZ-VOUS PREMIERE DEMANDE DE TITRE DE SEJOUR</t>
-  </si>
-  <si>
-    <t>PRISE DE RENDEZ-VOUS SAUF-CONDUITS</t>
-  </si>
-  <si>
-    <t>PRISE DE RENDEZ-VOUS RENOUVELLEMENT DE TITRE DE SEJOUR HORS ANEF</t>
-  </si>
-  <si>
-    <t>PRISE DE RENDEZ-VOUS RENOUVELLEMENT RECEPISSE</t>
-  </si>
-  <si>
-    <t>PRISE DE RENDEZ-VOUS REMISE DE TITRES</t>
-  </si>
-  <si>
-    <t>Le demandeur désire prendre un rendez-vous. La raison du rendez-vous est : remise de titre</t>
-  </si>
-  <si>
-    <t>Le demandeur sollicite la prise d'un rendez-vous pour le renouvellement de son récépissé</t>
-  </si>
-  <si>
-    <t>Le demandeur demande à prendre un rendez-vous pour le renouvellement d'un titre de séjour. Sa demande s'inscrit dans un processus géré en dehors du site de l'anef</t>
-  </si>
-  <si>
-    <t>Le demandeur demande à prendre un rendez-vous pour un sauf-conduit</t>
-  </si>
-  <si>
-    <t>Le demandeur demande à prendre un rendez-vous pour une première demande de titre de séjour</t>
-  </si>
-  <si>
-    <t>dublin</t>
-  </si>
-  <si>
-    <t>Your request related to your Dublin procedure</t>
-  </si>
-  <si>
-    <t>{prenom} {nom},
-We acknowledge receipt of your request dated {date_request} concerning your Dublin procedure.
-Yours sincerely,
-Migration and Integration Department
-Yvelines Prefecture</t>
-  </si>
-  <si>
-    <t>Procédure Dublin en cours</t>
+Préfecture des Yvelines
+Direction des migrations et de l'intégration</t>
   </si>
   <si>
     <t>{prenom} {nom},
@@ -1322,170 +1471,32 @@
 - la date des funérailles
 - votre carte de séjour
 - d'un justificatif de domicile de moins de 6 mois en indiquant en objet URGENT DEMANDE DE SAUF CONDUIT.
-En espérant vous avoir apporté les éléments souhaités,</t>
+En espérant vous avoir apporté les éléments souhaités,
+Préfecture des Yvelines
+Direction des migrations et de l'intégration</t>
   </si>
   <si>
     <t>{prenom} {nom},
-Nous accusons réception de votre demande du {date_demande} à propos de tudvotre procédure Dublin en cours.
+Nous accusons réception de votre demande du {date_demande} concernant l'expiration de votre Attestation de Demande d’Asile (ATDA).
 Nous vous prions d’agréer, {prenom} {nom}, l’expression de notre considération distinguée.
-Direction des migrations et de l'intégration
-Préfecture des Yvelines</t>
-  </si>
-  <si>
-    <t>asile_hebergement_urgence</t>
-  </si>
-  <si>
-    <t>aide_financiere_demandeur_asile</t>
-  </si>
-  <si>
-    <t>The applicant requests an appointment to submit an initial application for a residence permit.</t>
-  </si>
-  <si>
-    <t>The applicant wishes to return to their country for exceptional reasons (e.g. death of a relative, marriage of a relative, birth).</t>
-  </si>
-  <si>
-    <t>The applicant states that he wishes to apply for asylum.</t>
-  </si>
-  <si>
-    <t>DEMANDE D'AIDE FINANCIERE POUR UN DEMANDEUR D'ASILE</t>
-  </si>
-  <si>
-    <t>DEMANDE D'HEBERGEMENT D'URGENCE POUR UN DEMANDEUR D'ASILE</t>
-  </si>
-  <si>
-    <t>Le demandeur d'asile a besoin d'un hébergement d'urgence et en fait la demande</t>
-  </si>
-  <si>
-    <t>Le demandeur d'asile a besoin d'une aide financière et en fait la demande</t>
-  </si>
-  <si>
-    <t>APPLICATION FOR EMERGENCY ACCOMMODATION FOR AN ASYLUM SEEKER</t>
-  </si>
-  <si>
-    <t>APPLICATION FOR FINANCIAL ASSISTANCE FOR AN ASYLUM SEEKER</t>
-  </si>
-  <si>
-    <t>The asylum seeker requires emergency accommodation and has applied for it.</t>
-  </si>
-  <si>
-    <t>The asylum seeker requires financial assistance and is applying for it.</t>
-  </si>
-  <si>
-    <t>demandeur_d_asile</t>
-  </si>
-  <si>
-    <t>Demandeur d'asile</t>
-  </si>
-  <si>
-    <t>Asylum seeker</t>
-  </si>
-  <si>
-    <t>Le sauf-conduit est demandé pour motif de décès</t>
-  </si>
-  <si>
-    <t>demandeur d'asile</t>
-  </si>
-  <si>
-    <t>asylum seeker</t>
-  </si>
-  <si>
-    <t>aide_financiere_demandeur_asile asile_hebergement_urgence</t>
-  </si>
-  <si>
-    <t>RECEPISSE_VA_EXPIRER_DANS_X_JOURS</t>
-  </si>
-  <si>
-    <t>TITRE_SEJOUR_EXPIRE_DEPUIS_X_JOURS</t>
-  </si>
-  <si>
-    <t>TITRE_SEJOUR_VA_EXPIRER_DANS_X_JOURS</t>
-  </si>
-  <si>
-    <t>RELEVE_DE_L_ANEF</t>
-  </si>
-  <si>
-    <t>Please reach out to your contact at OFPRA or visit the[OFPRA website](https://www.usager.ofpra.gouv.fr/).</t>
-  </si>
-  <si>
-    <t>Veuillez vous adresser à votre contact OFPRA ou rendez-vous sur le site de l'[OFPRA](https://www.usager.ofpra.gouv.fr/).</t>
-  </si>
-  <si>
-    <t>Le récépissé va expirer dans {0} jour(s)</t>
-  </si>
-  <si>
-    <t>Le titre de séjour va expirer dans {0} jour(s)</t>
-  </si>
-  <si>
-    <t>Le titre de séjour est expiré depuis {0} jour(s)</t>
-  </si>
-  <si>
-    <t>L'API est expirée depuis {0} jour(s)</t>
-  </si>
-  <si>
-    <t>The receipt will expire in {0} day(s)</t>
-  </si>
-  <si>
-    <t>The residence permit will expire in {0} day(s)</t>
-  </si>
-  <si>
-    <t>The residence permit expired {0} day(s) ago</t>
-  </si>
-  <si>
-    <t>Relève de l'ANEF</t>
-  </si>
-  <si>
-    <t>Reports to ANEF</t>
-  </si>
-  <si>
-    <t>DEMANDEUR_D_ASILE</t>
-  </si>
-  <si>
-    <t>Est demadeur d'asile</t>
-  </si>
-  <si>
-    <t>Is an asylum seeker</t>
-  </si>
-  <si>
-    <t>STATUT</t>
-  </si>
-  <si>
-    <t>A déclaré le statut : {0}</t>
-  </si>
-  <si>
-    <t>Status is {0}</t>
-  </si>
-  <si>
-    <t>Si vous êtes sans solution, appeler le 115 pour trouver un hébergement d'urgence (appel gratuit).</t>
-  </si>
-  <si>
-    <t>If you are unable to find a solution, call 115 to find emergency accommodation (free call).</t>
-  </si>
-  <si>
-    <t>APPEL_115</t>
-  </si>
-  <si>
-    <t>AUCUNE_SOLUTION</t>
-  </si>
-  <si>
-    <t>La préfecture n'a aucune solution à vous proposer et nous en sommes désolés.</t>
-  </si>
-  <si>
-    <t>The prefecture has no solution to offer you, and we are sorry about that.</t>
-  </si>
-  <si>
-    <t>DEMANDE DE DUPLICATA</t>
-  </si>
-  <si>
-    <t>Le demandeur a besoin d'un duplicata</t>
-  </si>
-  <si>
-    <t>REQUEST FOR DUPLICATE</t>
-  </si>
-  <si>
-    <t>The applicant requires a duplicate copy.</t>
-  </si>
-  <si>
-    <t>duplicata</t>
+Préfecture des Yvelines
+Direction des migrations et de l'intégration</t>
+  </si>
+  <si>
+    <t>{prenom} {nom},
+Nous accusons réception de votre demande du {date_demande} à propos de votre procédure Dublin en cours.
+Nous vous prions d’agréer, {prenom} {nom}, l’expression de notre considération distinguée.
+Préfecture des Yvelines
+Direction des migrations et de l'intégration</t>
+  </si>
+  <si>
+    <t>numero_dossier_ANEF</t>
+  </si>
+  <si>
+    <t>Numéro de dossier ANEF</t>
+  </si>
+  <si>
+    <t>ANEF file number</t>
   </si>
   <si>
     <t>pref-delphes-sejour@yvelines.gouv.fr,pref-delphes-asile@yvelines.gouv.fr</t>
@@ -1681,7 +1692,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1720,6 +1730,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="2" quotePrefix="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Lien hypertexte" xfId="2" builtinId="8"/>
@@ -2093,7 +2104,7 @@
         <v>155</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>9</v>
@@ -2382,7 +2393,7 @@
         <v>172</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>26</v>
@@ -2392,156 +2403,156 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="51" x14ac:dyDescent="0.2">
-      <c r="A25" s="33" t="s">
+      <c r="A25" s="32" t="s">
+        <v>348</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>349</v>
+      </c>
+      <c r="E25" s="28" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A26" s="32" t="s">
         <v>351</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B26" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>359</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="D26" s="28" t="s">
+        <v>392</v>
+      </c>
+      <c r="E26" s="28" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A27" s="32" t="s">
+        <v>352</v>
+      </c>
+      <c r="B27" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="D25" s="24" t="s">
-        <v>352</v>
-      </c>
-      <c r="E25" s="29" t="s">
+      <c r="C27" s="2" t="s">
+        <v>361</v>
+      </c>
+      <c r="D27" s="28" t="s">
+        <v>391</v>
+      </c>
+      <c r="E27" s="28" t="s">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="68" x14ac:dyDescent="0.2">
+      <c r="A28" s="32" t="s">
         <v>353</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A26" s="33" t="s">
+      <c r="B28" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="D28" s="28" t="s">
+        <v>390</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A29" s="32" t="s">
         <v>354</v>
       </c>
-      <c r="B26" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="D26" s="29" t="s">
-        <v>395</v>
-      </c>
-      <c r="E26" s="29" t="s">
+      <c r="B29" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="D29" s="28" t="s">
+        <v>389</v>
+      </c>
+      <c r="E29" s="28" t="s">
         <v>396</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A27" s="33" t="s">
+    <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.2">
+      <c r="A30" s="32" t="s">
         <v>355</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="D27" s="29" t="s">
-        <v>394</v>
-      </c>
-      <c r="E27" s="29" t="s">
+      <c r="B30" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="D30" s="28" t="s">
+        <v>388</v>
+      </c>
+      <c r="E30" s="28" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="68" x14ac:dyDescent="0.2">
-      <c r="A28" s="33" t="s">
-        <v>356</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="D28" s="29" t="s">
-        <v>393</v>
-      </c>
-      <c r="E28" s="29" t="s">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A29" s="33" t="s">
-        <v>357</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="D29" s="29" t="s">
-        <v>392</v>
-      </c>
-      <c r="E29" s="29" t="s">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" ht="34" x14ac:dyDescent="0.2">
-      <c r="A30" s="33" t="s">
-        <v>358</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="C30" s="2" t="s">
+    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="31" t="s">
+        <v>402</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>411</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>413</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="D30" s="29" t="s">
-        <v>391</v>
-      </c>
-      <c r="E30" s="29" t="s">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A31" s="32" t="s">
+    </row>
+    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+      <c r="A32" s="31" t="s">
+        <v>403</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="B31" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" ht="32" x14ac:dyDescent="0.2">
-      <c r="A32" s="32" t="s">
-        <v>408</v>
-      </c>
-      <c r="B32" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>412</v>
-      </c>
       <c r="E32" s="2" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="5" t="s">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>457</v>
-      </c>
-      <c r="D33" s="36" t="s">
-        <v>454</v>
-      </c>
-      <c r="E33" s="36" t="s">
-        <v>455</v>
+        <v>452</v>
+      </c>
+      <c r="D33" s="35" t="s">
+        <v>449</v>
+      </c>
+      <c r="E33" s="35" t="s">
+        <v>450</v>
       </c>
     </row>
   </sheetData>
@@ -2632,10 +2643,10 @@
       <c r="B3" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>259</v>
       </c>
       <c r="E3" s="14" t="s">
@@ -2652,16 +2663,16 @@
       <c r="B4" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="D4" s="18" t="s">
+      <c r="D4" s="17" t="s">
         <v>260</v>
       </c>
       <c r="E4" s="14" t="s">
         <v>240</v>
       </c>
-      <c r="F4" s="21" t="s">
+      <c r="F4" s="20" t="s">
         <v>255</v>
       </c>
     </row>
@@ -2697,7 +2708,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B2" sqref="B2:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2732,7 +2743,7 @@
         <v>93</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -2785,8 +2796,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{EA35456F-8910-A447-A530-A1B5920653C2}"/>
-    <hyperlink ref="B3" r:id="rId2" xr:uid="{DF713DBF-8911-1849-A5C8-8B9A05AD0BE3}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{819B9DBF-2DEB-814B-88AB-7640294ADBFC}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{E6110F30-809C-CA48-9D9D-06BCB1E42556}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
@@ -2797,7 +2808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAADDD23-DB13-4EC8-8D22-BE27FCA5478C}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
+    <sheetView topLeftCell="B3" workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
@@ -2827,7 +2838,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="350" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="365" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>99</v>
       </c>
@@ -2841,10 +2852,10 @@
         <v>82</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="160" x14ac:dyDescent="0.2">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>100</v>
       </c>
@@ -2858,41 +2869,41 @@
         <v>101</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="160" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="128" x14ac:dyDescent="0.2">
-      <c r="A5" s="30" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="144" x14ac:dyDescent="0.2">
+      <c r="A5" s="29" t="s">
+        <v>398</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>399</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="D5" s="29" t="s">
         <v>401</v>
       </c>
-      <c r="B5" s="30" t="s">
-        <v>402</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="D5" s="30" t="s">
-        <v>404</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>406</v>
+        <v>458</v>
       </c>
     </row>
   </sheetData>
@@ -2923,14 +2934,14 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView zoomScale="184" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A16"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="40.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.33203125" bestFit="1" customWidth="1"/>
   </cols>
@@ -2954,13 +2965,13 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D2" s="7" t="s">
         <v>232</v>
@@ -2971,13 +2982,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C3" s="7" t="s">
-        <v>313</v>
+        <v>454</v>
       </c>
       <c r="D3" s="7" t="s">
         <v>232</v>
@@ -2988,13 +2999,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="7" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>232</v>
@@ -3005,13 +3016,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D5" s="7" t="s">
         <v>232</v>
@@ -3022,13 +3033,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>232</v>
@@ -3039,13 +3050,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>232</v>
@@ -3056,13 +3067,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D8" s="7" t="s">
         <v>232</v>
@@ -3073,13 +3084,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D9" s="7" t="s">
         <v>232</v>
@@ -3090,13 +3101,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="7" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D10" s="7" t="s">
         <v>232</v>
@@ -3107,13 +3118,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="7" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D11" s="7" t="s">
         <v>232</v>
@@ -3124,13 +3135,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="7" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D12" s="7" t="s">
         <v>232</v>
@@ -3141,13 +3152,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D13" s="7" t="s">
         <v>232</v>
@@ -3158,13 +3169,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D14" s="7" t="s">
         <v>232</v>
@@ -3175,13 +3186,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="7" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D15" s="7" t="s">
         <v>232</v>
@@ -3192,13 +3203,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>232</v>
@@ -3209,13 +3220,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>341</v>
+      </c>
+      <c r="C17" s="7" t="s">
         <v>342</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>343</v>
-      </c>
-      <c r="C17" s="7" t="s">
-        <v>344</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>232</v>
@@ -3536,12 +3547,12 @@
       <c r="D19" s="7" t="s">
         <v>285</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="21" t="s">
         <v>286</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="H31" s="20"/>
+      <c r="H31" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3738,7 +3749,7 @@
         <v>197</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>436</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="16" x14ac:dyDescent="0.2">
@@ -3754,68 +3765,68 @@
     </row>
     <row r="5" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>433</v>
+        <v>428</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>435</v>
+        <v>430</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="C7" s="7" t="s">
         <v>429</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>438</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
+        <v>437</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>439</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="34" t="s">
+        <v>440</v>
+      </c>
+      <c r="B10" s="25" t="s">
         <v>442</v>
       </c>
-      <c r="B9" s="7" t="s">
-        <v>444</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="35" t="s">
-        <v>445</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>447</v>
-      </c>
-      <c r="C10" s="26" t="s">
-        <v>446</v>
+      <c r="C10" s="25" t="s">
+        <v>441</v>
       </c>
     </row>
   </sheetData>
@@ -3859,10 +3870,10 @@
         <v>188</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>376</v>
+        <v>373</v>
       </c>
       <c r="D2" s="2"/>
     </row>
@@ -3871,10 +3882,10 @@
         <v>193</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>378</v>
+        <v>375</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>195</v>
@@ -3885,46 +3896,46 @@
         <v>192</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>374</v>
+        <v>371</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>375</v>
+        <v>372</v>
       </c>
       <c r="D5" s="5"/>
     </row>
     <row r="6" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="D6" s="5"/>
     </row>
     <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="D7" s="7"/>
     </row>
@@ -3936,10 +3947,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF16B1B1-A6B4-4B56-9813-CCF1B731EDAC}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:Q17"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M16" sqref="M16"/>
+    <sheetView topLeftCell="C1" zoomScale="137" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4015,10 +4026,10 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>105</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -4068,10 +4079,10 @@
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="7" t="s">
@@ -4121,10 +4132,10 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C4" s="7" t="s">
@@ -4174,10 +4185,10 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="7" t="s">
@@ -4227,10 +4238,10 @@
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -4280,10 +4291,10 @@
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -4295,10 +4306,10 @@
       <c r="E7" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="36" t="s">
         <v>115</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="36" t="s">
         <v>115</v>
       </c>
       <c r="H7" s="14" t="s">
@@ -4333,10 +4344,10 @@
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="16" t="s">
         <v>4</v>
       </c>
       <c r="C8" s="7" t="s">
@@ -4386,10 +4397,10 @@
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="16" t="s">
         <v>105</v>
       </c>
       <c r="C9" s="7" t="s">
@@ -4439,10 +4450,10 @@
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A10" s="17" t="s">
+      <c r="A10" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C10" s="7" t="s">
@@ -4492,10 +4503,10 @@
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="B11" s="17" t="s">
+      <c r="B11" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -4545,35 +4556,35 @@
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="16" t="s">
+        <v>293</v>
+      </c>
+      <c r="B12" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="B12" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="7" t="s">
         <v>295</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="F12" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="H12" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="I12" s="14" t="s">
+        <v>339</v>
+      </c>
+      <c r="J12" s="14" t="s">
         <v>296</v>
-      </c>
-      <c r="E12" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="G12" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>240</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>341</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>297</v>
       </c>
       <c r="K12" s="8" t="s">
         <v>288</v>
@@ -4582,7 +4593,7 @@
         <v>232</v>
       </c>
       <c r="M12" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="N12" s="8" t="s">
         <v>240</v>
@@ -4598,35 +4609,35 @@
       </c>
     </row>
     <row r="13" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="25" t="s">
-        <v>370</v>
-      </c>
-      <c r="B13" s="25" t="s">
+      <c r="A13" s="24" t="s">
+        <v>367</v>
+      </c>
+      <c r="B13" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C13" s="26" t="s">
-        <v>372</v>
-      </c>
-      <c r="D13" s="26" t="s">
-        <v>371</v>
-      </c>
-      <c r="E13" s="27" t="s">
+      <c r="C13" s="25" t="s">
+        <v>369</v>
+      </c>
+      <c r="D13" s="25" t="s">
+        <v>368</v>
+      </c>
+      <c r="E13" s="26" t="s">
         <v>233</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>288</v>
       </c>
-      <c r="L13" s="27" t="s">
-        <v>232</v>
-      </c>
-      <c r="M13" s="23" t="s">
-        <v>357</v>
+      <c r="L13" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="M13" s="22" t="s">
+        <v>354</v>
       </c>
       <c r="N13" t="s">
-        <v>373</v>
-      </c>
-      <c r="O13" s="26" t="s">
-        <v>423</v>
+        <v>370</v>
+      </c>
+      <c r="O13" s="25" t="s">
+        <v>418</v>
       </c>
       <c r="P13" s="7" t="s">
         <v>76</v>
@@ -4636,17 +4647,17 @@
       </c>
     </row>
     <row r="14" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="17" t="s">
-        <v>381</v>
-      </c>
-      <c r="B14" s="17" t="s">
+      <c r="A14" s="16" t="s">
+        <v>378</v>
+      </c>
+      <c r="B14" s="16" t="s">
         <v>105</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>233</v>
@@ -4672,14 +4683,14 @@
       <c r="L14" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="M14" s="28" t="s">
-        <v>355</v>
+      <c r="M14" s="27" t="s">
+        <v>352</v>
       </c>
       <c r="N14" s="7" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="O14" s="7" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="P14" s="7" t="s">
         <v>76</v>
@@ -4689,17 +4700,17 @@
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="A15" s="17" t="s">
-        <v>386</v>
-      </c>
-      <c r="B15" s="17" t="s">
+      <c r="A15" s="16" t="s">
+        <v>383</v>
+      </c>
+      <c r="B15" s="16" t="s">
         <v>105</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>233</v>
@@ -4726,13 +4737,13 @@
         <v>232</v>
       </c>
       <c r="M15" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="O15" s="7" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="P15" s="7" t="s">
         <v>76</v>
@@ -4742,17 +4753,17 @@
       </c>
     </row>
     <row r="16" spans="1:17" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="17" t="s">
-        <v>420</v>
-      </c>
-      <c r="B16" s="17" t="s">
+      <c r="A16" s="16" t="s">
+        <v>415</v>
+      </c>
+      <c r="B16" s="16" t="s">
         <v>5</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="D16" s="7" t="s">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>233</v>
@@ -4768,20 +4779,67 @@
       <c r="L16" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="M16" s="31" t="s">
-        <v>426</v>
-      </c>
-      <c r="N16" s="34" t="s">
-        <v>425</v>
-      </c>
-      <c r="O16" s="26" t="s">
-        <v>424</v>
+      <c r="M16" s="30" t="s">
+        <v>421</v>
+      </c>
+      <c r="N16" s="33" t="s">
+        <v>420</v>
+      </c>
+      <c r="O16" s="25" t="s">
+        <v>419</v>
       </c>
       <c r="P16" s="7" t="s">
         <v>76</v>
       </c>
       <c r="Q16" s="8" t="s">
         <v>232</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A17" s="16" t="s">
+        <v>459</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="E17" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="I17" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8" t="s">
+        <v>288</v>
+      </c>
+      <c r="L17" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="N17" s="7" t="s">
+        <v>461</v>
+      </c>
+      <c r="O17" s="7" t="s">
+        <v>460</v>
+      </c>
+      <c r="P17" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q17" s="8" t="s">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -4930,7 +4988,7 @@
         <v>220</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16" x14ac:dyDescent="0.2">

</xml_diff>